<commit_message>
# Creating multiple feature files
</commit_message>
<xml_diff>
--- a/CaddyCode/src/test/resources/TestData/Testdata.xlsx
+++ b/CaddyCode/src/test/resources/TestData/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="11700" windowHeight="3360"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11340" windowHeight="1770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>Reddy</t>
   </si>
@@ -230,16 +230,13 @@
     <t>PhoneNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">Ganesh </t>
-  </si>
-  <si>
-    <t>Shetty</t>
-  </si>
-  <si>
-    <t>Ganesh9796</t>
-  </si>
-  <si>
-    <t>prasad898587@yopmail.com</t>
+    <t>venkat</t>
+  </si>
+  <si>
+    <t>prasad8985117@yopmail.com</t>
+  </si>
+  <si>
+    <t>Ganesh979612</t>
   </si>
 </sst>
 </file>
@@ -625,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -697,10 +694,10 @@
         <v>70</v>
       </c>
       <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Updated generic and feature
</commit_message>
<xml_diff>
--- a/CaddyCode/src/test/resources/TestData/Testdata.xlsx
+++ b/CaddyCode/src/test/resources/TestData/Testdata.xlsx
@@ -233,10 +233,10 @@
     <t>venkat</t>
   </si>
   <si>
-    <t>Ganesh9796123</t>
-  </si>
-  <si>
-    <t>prasad89851137@yopmail.com</t>
+    <t>prasad868927@yopmail.com</t>
+  </si>
+  <si>
+    <t>Ganesh998</t>
   </si>
 </sst>
 </file>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -697,13 +697,13 @@
         <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F7" s="7">
         <v>98457895463</v>

</xml_diff>